<commit_message>
[feat]: excel download routes added
</commit_message>
<xml_diff>
--- a/data/generated/hr_leave_applications.xlsx
+++ b/data/generated/hr_leave_applications.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -451,148 +451,54 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v/>
+        <v>LV-1753795678579-DDHA</v>
       </c>
       <c r="B2" t="str">
-        <v/>
+        <v>Manager</v>
       </c>
       <c r="C2" t="str">
-        <v/>
+        <v>PILLP305</v>
       </c>
       <c r="D2" t="str">
-        <v/>
-      </c>
-      <c r="E2" t="str">
-        <v/>
+        <v>Animesh Roy</v>
+      </c>
+      <c r="E2">
+        <v>8145312848</v>
       </c>
       <c r="F2" t="str">
-        <v/>
+        <v>animesh.roy@pillp.in</v>
       </c>
       <c r="G2" t="str">
-        <v/>
+        <v>Mechanical HOD</v>
       </c>
       <c r="H2" t="str">
-        <v/>
+        <v>Mechanical</v>
       </c>
       <c r="I2" t="str">
-        <v/>
+        <v>Raichur</v>
       </c>
       <c r="J2" t="str">
-        <v/>
+        <v>02-12-2025</v>
       </c>
       <c r="K2" t="str">
-        <v/>
+        <v>07-12-2025</v>
       </c>
       <c r="L2" t="str">
-        <v/>
+        <v>For my personal reason</v>
       </c>
       <c r="M2" t="str">
-        <v/>
+        <v>Pending</v>
       </c>
       <c r="N2" t="str">
-        <v/>
+        <v>2025-07-29</v>
       </c>
       <c r="O2" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>LV-1753526987168-INVG</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Manager</v>
-      </c>
-      <c r="C3" t="str">
-        <v>PILLP399</v>
-      </c>
-      <c r="D3" t="str">
-        <v>Deepchayan Roy Chowdhury</v>
-      </c>
-      <c r="E3">
-        <v>8145312848</v>
-      </c>
-      <c r="F3" t="str">
-        <v>deepchayan.chowdhury@pillp.in</v>
-      </c>
-      <c r="G3" t="str">
-        <v xml:space="preserve">HR Executive </v>
-      </c>
-      <c r="H3" t="str">
-        <v>Human Resource</v>
-      </c>
-      <c r="I3" t="str">
-        <v>All</v>
-      </c>
-      <c r="J3" t="str">
-        <v>02-12-2025</v>
-      </c>
-      <c r="K3" t="str">
-        <v>07-12-2025</v>
-      </c>
-      <c r="L3" t="str">
-        <v>For my personal reason</v>
-      </c>
-      <c r="M3" t="str">
-        <v>Pending</v>
-      </c>
-      <c r="N3" t="str">
-        <v>2025-07-26</v>
-      </c>
-      <c r="O3" t="str">
-        <v>2025-07-26</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>LV-1753528055049-S2BW</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Manager</v>
-      </c>
-      <c r="C4" t="str">
-        <v>PILLP305</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Animesh Roy</v>
-      </c>
-      <c r="E4">
-        <v>8145312848</v>
-      </c>
-      <c r="F4" t="str">
-        <v>animesh.roy@pillp.in</v>
-      </c>
-      <c r="G4" t="str">
-        <v>Mechanical HOD</v>
-      </c>
-      <c r="H4" t="str">
-        <v>Mechanical</v>
-      </c>
-      <c r="I4" t="str">
-        <v>Raichur</v>
-      </c>
-      <c r="J4" t="str">
-        <v>02-12-2025</v>
-      </c>
-      <c r="K4" t="str">
-        <v>07-12-2025</v>
-      </c>
-      <c r="L4" t="str">
-        <v>For my personal reason</v>
-      </c>
-      <c r="M4" t="str">
-        <v>Pending</v>
-      </c>
-      <c r="N4" t="str">
-        <v>2025-07-26</v>
-      </c>
-      <c r="O4" t="str">
-        <v>2025-07-26</v>
+        <v>2025-07-29</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: hr-manager controller is little modified
</commit_message>
<xml_diff>
--- a/data/generated/hr_leave_applications.xlsx
+++ b/data/generated/hr_leave_applications.xlsx
@@ -1,41 +1,77 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\JavaScript Projects\leave-management-system\data\generated\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B5C265-27AA-4816-8E69-009CDE887A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>Leave ID</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Employee Code</t>
+  </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>WhatsApp Number</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Work Location</t>
+  </si>
+  <si>
+    <t>From Date</t>
+  </si>
+  <si>
+    <t>To Date</t>
+  </si>
+  <si>
+    <t>Leave Reason</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Submission Date</t>
+  </si>
+  <si>
+    <t>Last Updated</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,13 +101,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,109 +440,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Leave ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Role</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Employee Code</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Employee Name</v>
-      </c>
-      <c r="E1" t="str">
-        <v>WhatsApp Number</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Email</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Designation</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Department</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Work Location</v>
-      </c>
-      <c r="J1" t="str">
-        <v>From Date</v>
-      </c>
-      <c r="K1" t="str">
-        <v>To Date</v>
-      </c>
-      <c r="L1" t="str">
-        <v>Leave Reason</v>
-      </c>
-      <c r="M1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="N1" t="str">
-        <v>Submission Date</v>
-      </c>
-      <c r="O1" t="str">
-        <v>Last Updated</v>
+    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>LV-1753795678579-DDHA</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Manager</v>
-      </c>
-      <c r="C2" t="str">
-        <v>PILLP305</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Animesh Roy</v>
-      </c>
-      <c r="E2">
-        <v>8145312848</v>
-      </c>
-      <c r="F2" t="str">
-        <v>animesh.roy@pillp.in</v>
-      </c>
-      <c r="G2" t="str">
-        <v>Mechanical HOD</v>
-      </c>
-      <c r="H2" t="str">
-        <v>Mechanical</v>
-      </c>
-      <c r="I2" t="str">
-        <v>Raichur</v>
-      </c>
-      <c r="J2" t="str">
-        <v>02-12-2025</v>
-      </c>
-      <c r="K2" t="str">
-        <v>07-12-2025</v>
-      </c>
-      <c r="L2" t="str">
-        <v>For my personal reason</v>
-      </c>
-      <c r="M2" t="str">
-        <v>Pending</v>
-      </c>
-      <c r="N2" t="str">
-        <v>2025-07-29</v>
-      </c>
-      <c r="O2" t="str">
-        <v>2025-07-29</v>
-      </c>
-    </row>
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O2"/>
+    <ignoredError sqref="A1:O1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
patch: date formatting fixed
</commit_message>
<xml_diff>
--- a/data/generated/hr_leave_applications.xlsx
+++ b/data/generated/hr_leave_applications.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\JavaScript Projects\leave-management-system\data\generated\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B5C265-27AA-4816-8E69-009CDE887A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -70,10 +64,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -100,20 +95,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -124,10 +122,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -165,71 +163,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -253,50 +251,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -306,7 +307,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -315,7 +316,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -324,7 +325,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -332,10 +333,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -364,7 +365,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -377,13 +378,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -395,113 +395,87 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:O1" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>